<commit_message>
Some Documents are ready.
</commit_message>
<xml_diff>
--- a/DOC/Gantt_Chart_BMI.xlsx
+++ b/DOC/Gantt_Chart_BMI.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cem\Documents\YandexDisk\Boğaziçi dersler\SWE 573\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cem\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -431,7 +431,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>BMI Calculator Project Schedule</t>
   </si>
@@ -544,6 +544,21 @@
   </si>
   <si>
     <t>Finding the working and full Spring IDE.</t>
+  </si>
+  <si>
+    <t>revision milestone</t>
+  </si>
+  <si>
+    <t>estimated time</t>
+  </si>
+  <si>
+    <t>actual time</t>
+  </si>
+  <si>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <t>project libre</t>
   </si>
 </sst>
 </file>
@@ -755,7 +770,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -849,6 +864,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1165,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1196,7 @@
     <col min="5" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1186,12 +1204,12 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="31" t="s">
         <v>2</v>
@@ -1203,7 +1221,7 @@
       </c>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="31" t="s">
         <v>4</v>
@@ -1215,7 +1233,7 @@
       </c>
       <c r="F4" s="33"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="34" t="s">
         <v>5</v>
@@ -1227,7 +1245,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="26"/>
       <c r="C6" s="25"/>
@@ -1242,17 +1260,17 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
@@ -1278,8 +1296,17 @@
         <v>11</v>
       </c>
       <c r="I9" s="13"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="L9" s="35" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="str">
         <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A10,-1,0,1,1),".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A10,-1,0,1,1),".","`",1))),TEXT(VALUE(OFFSET(A10,-1,0,1,1))+1,"#"),TEXT(VALUE(LEFT(OFFSET(A10,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A10,-1,0,1,1),".","`",1))-1))+1,"#")))</f>
         <v>1</v>
@@ -1290,7 +1317,7 @@
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="str">
         <f t="shared" ref="A11:A19" ca="1" si="0">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A11,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A11,-1,0,1,1),".","`",1))),OFFSET(A11,-1,0,1,1)&amp;".1",LEFT(OFFSET(A11,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A11,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A11,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A11,-1,0,1,1),LEN(OFFSET(A11,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A11,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A11,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A11,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A11,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A11,-1,0,1,1),".","`",1))-1)))+1)))</f>
         <v>1.1</v>
@@ -1315,7 +1342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>1.2</v>
@@ -1340,7 +1367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>1.3</v>
@@ -1365,7 +1392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>1.4</v>
@@ -1390,7 +1417,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>1.5</v>
@@ -1415,7 +1442,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>1.6</v>
@@ -1440,7 +1467,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>1.7</v>
@@ -1465,7 +1492,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>1.8</v>
@@ -1490,7 +1517,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>1.9</v>
@@ -1514,7 +1541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="str">
         <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A20,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A20,-1,0,1,1),".","`",1))),OFFSET(A20,-1,0,1,1)&amp;".1",LEFT(OFFSET(A20,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A20,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A20,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A20,-1,0,1,1),LEN(OFFSET(A20,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A20,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A20,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A20,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A20,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A20,-1,0,1,1),".","`",1))-1)))+1)))</f>
         <v>1.10</v>
@@ -1535,7 +1562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="str">
         <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(OFFSET(A21,-1,0,1,1),".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))),OFFSET(A21,-1,0,1,1)&amp;".1",LEFT(OFFSET(A21,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",2))),VALUE(RIGHT(OFFSET(A21,-1,0,1,1),LEN(OFFSET(A21,-1,0,1,1))-FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))))+1,VALUE(MID(OFFSET(A21,-1,0,1,1),FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))+1,(FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",2))-FIND("`",SUBSTITUTE(OFFSET(A21,-1,0,1,1),".","`",1))-1)))+1)))</f>
         <v>1.11</v>
@@ -1558,8 +1585,14 @@
       <c r="H21" s="22">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>37</v>
+      </c>
+      <c r="M21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="14"/>
       <c r="B24" s="15" t="s">
         <v>27</v>

</xml_diff>